<commit_message>
formatting add leavequota Leavetypes to luis
</commit_message>
<xml_diff>
--- a/sitLeaveTypes.xlsx
+++ b/sitLeaveTypes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyNodejs\Chatbot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D43326-5D62-4245-A520-A9CEAD8A6835}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00781A21-87D6-4782-AE4C-5A0F823469CA}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{14F76CCE-F77F-4AD6-B333-89D63F913CD1}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="68">
   <si>
     <t>Leave Type</t>
   </si>
@@ -191,9 +191,6 @@
   </si>
   <si>
     <t>Child Care Leave</t>
-  </si>
-  <si>
-    <t>Ext Maternity (UP-Non- SC)</t>
   </si>
   <si>
     <t>Unpaid Infant Care Leave</t>
@@ -615,11 +612,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69CFDCB5-896E-435E-AEF6-7DDDF4E1DBC9}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -685,7 +688,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
@@ -967,7 +970,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -982,7 +985,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -993,7 +996,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
@@ -1004,7 +1007,7 @@
         <v>52</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
@@ -1015,7 +1018,7 @@
         <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
@@ -1111,7 +1114,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="B13" s="1">
         <v>28</v>
@@ -1144,7 +1147,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B16" s="1">
         <v>33</v>
@@ -1155,7 +1158,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B17" s="1">
         <v>36</v>
@@ -1177,7 +1180,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B19" s="1">
         <v>41</v>
@@ -1188,7 +1191,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B20" s="1">
         <v>42</v>
@@ -1199,7 +1202,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B21" s="1">
         <v>43</v>
@@ -1210,7 +1213,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B22" s="1">
         <v>44</v>
@@ -1232,7 +1235,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B24" s="1">
         <v>52</v>
@@ -1254,7 +1257,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B26" s="1">
         <v>80</v>
@@ -1265,7 +1268,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B27" s="1">
         <v>81</v>

</xml_diff>